<commit_message>
correct cvd and muskuloskeletal harmo rule (NA_integer_)
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHK.xlsx
+++ b/data_processing_elements-CHK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD7E8BC-6EF1-499C-AD63-9AD93515C8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9C9C79-9A4C-4756-8D6F-D15D0559BEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DEB00B6D-B98D-41B0-8753-944EECEBCC27}"/>
   </bookViews>
@@ -835,12 +835,6 @@
     <t>case_when</t>
   </si>
   <si>
-    <t>case_when(
-MHSTRK == 1 | MHHEART == 1 | MHBP == 1 ~ 1L;
-MHSTRK == 0 &amp; MHHEART == 0 &amp; MHBP == 0 ~ 0L;
-ELSE ~ NA_integer)</t>
-  </si>
-  <si>
     <t>could produce cat no because Medical History - Other Heart Disease</t>
   </si>
   <si>
@@ -862,11 +856,6 @@
   </si>
   <si>
     <t>The category "No" was not produced. Collected information included arthritis, osteoarthritis and osteoporosis.</t>
-  </si>
-  <si>
-    <t>case_when(
-MHART == 1 | MHOSTEO == 1 ~ 1L;
-ELSE ~ NA_integer)</t>
   </si>
   <si>
     <t>dis_diabetes</t>
@@ -1278,6 +1267,17 @@
   </si>
   <si>
     <t>information provided by the study</t>
+  </si>
+  <si>
+    <t>case_when(
+MHART == 1 | MHOSTEO == 1 ~ 1L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+MHSTRK == 1 | MHHEART == 1 | MHBP == 1 ~ 1L;
+MHSTRK == 0 &amp; MHHEART == 0 &amp; MHBP == 0 ~ 0L;
+ELSE ~ NA_integer_)</t>
   </si>
 </sst>
 </file>
@@ -1327,14 +1327,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1671,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90857538-AC28-4A1B-9DA3-1B4B03EDEFF4}">
   <dimension ref="A1:AD84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L68" sqref="L68"/>
+    <sheetView tabSelected="1" topLeftCell="H47" workbookViewId="0">
+      <selection activeCell="W49" sqref="W49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,7 +2329,7 @@
         <v>57</v>
       </c>
       <c r="W14" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -2365,13 +2364,13 @@
         <v>38</v>
       </c>
       <c r="V15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="W15">
         <v>2</v>
       </c>
       <c r="X15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -2591,7 +2590,7 @@
         <v>48</v>
       </c>
       <c r="W20" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -2749,10 +2748,10 @@
         <v>38</v>
       </c>
       <c r="V24" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="W24" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -2950,16 +2949,16 @@
       <c r="J29" t="s">
         <v>76</v>
       </c>
-      <c r="T29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U29" s="4" t="s">
+      <c r="T29" t="s">
+        <v>70</v>
+      </c>
+      <c r="U29" t="s">
         <v>77</v>
       </c>
-      <c r="V29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W29" s="4" t="s">
+      <c r="V29" t="s">
+        <v>70</v>
+      </c>
+      <c r="W29" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2988,16 +2987,16 @@
       <c r="J30" t="s">
         <v>76</v>
       </c>
-      <c r="T30" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U30" s="4" t="s">
+      <c r="T30" t="s">
+        <v>70</v>
+      </c>
+      <c r="U30" t="s">
         <v>77</v>
       </c>
-      <c r="V30" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W30" s="4" t="s">
+      <c r="V30" t="s">
+        <v>70</v>
+      </c>
+      <c r="W30" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3026,16 +3025,16 @@
       <c r="J31" t="s">
         <v>76</v>
       </c>
-      <c r="T31" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U31" s="4" t="s">
+      <c r="T31" t="s">
+        <v>70</v>
+      </c>
+      <c r="U31" t="s">
         <v>77</v>
       </c>
-      <c r="V31" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W31" s="4" t="s">
+      <c r="V31" t="s">
+        <v>70</v>
+      </c>
+      <c r="W31" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3064,16 +3063,16 @@
       <c r="J32" t="s">
         <v>76</v>
       </c>
-      <c r="T32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U32" s="4" t="s">
+      <c r="T32" t="s">
+        <v>70</v>
+      </c>
+      <c r="U32" t="s">
         <v>77</v>
       </c>
-      <c r="V32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W32" s="4" t="s">
+      <c r="V32" t="s">
+        <v>70</v>
+      </c>
+      <c r="W32" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3102,16 +3101,16 @@
       <c r="J33" t="s">
         <v>76</v>
       </c>
-      <c r="T33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U33" s="4" t="s">
+      <c r="T33" t="s">
+        <v>70</v>
+      </c>
+      <c r="U33" t="s">
         <v>77</v>
       </c>
-      <c r="V33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W33" s="4" t="s">
+      <c r="V33" t="s">
+        <v>70</v>
+      </c>
+      <c r="W33" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3140,16 +3139,16 @@
       <c r="J34" t="s">
         <v>76</v>
       </c>
-      <c r="T34" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U34" s="4" t="s">
+      <c r="T34" t="s">
+        <v>70</v>
+      </c>
+      <c r="U34" t="s">
         <v>77</v>
       </c>
-      <c r="V34" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W34" s="4" t="s">
+      <c r="V34" t="s">
+        <v>70</v>
+      </c>
+      <c r="W34" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3178,16 +3177,16 @@
       <c r="J35" t="s">
         <v>76</v>
       </c>
-      <c r="T35" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U35" s="4" t="s">
+      <c r="T35" t="s">
+        <v>70</v>
+      </c>
+      <c r="U35" t="s">
         <v>77</v>
       </c>
-      <c r="V35" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W35" s="4" t="s">
+      <c r="V35" t="s">
+        <v>70</v>
+      </c>
+      <c r="W35" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3216,16 +3215,16 @@
       <c r="J36" t="s">
         <v>76</v>
       </c>
-      <c r="T36" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U36" s="4" t="s">
+      <c r="T36" t="s">
+        <v>70</v>
+      </c>
+      <c r="U36" t="s">
         <v>77</v>
       </c>
-      <c r="V36" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W36" s="4" t="s">
+      <c r="V36" t="s">
+        <v>70</v>
+      </c>
+      <c r="W36" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3254,16 +3253,16 @@
       <c r="J37" t="s">
         <v>76</v>
       </c>
-      <c r="T37" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U37" s="4" t="s">
+      <c r="T37" t="s">
+        <v>70</v>
+      </c>
+      <c r="U37" t="s">
         <v>77</v>
       </c>
-      <c r="V37" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W37" s="4" t="s">
+      <c r="V37" t="s">
+        <v>70</v>
+      </c>
+      <c r="W37" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3539,7 +3538,7 @@
         <v>57</v>
       </c>
       <c r="W44" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="X44" t="s">
         <v>221</v>
@@ -3724,7 +3723,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="255" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="240" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3768,10 +3767,10 @@
         <v>252</v>
       </c>
       <c r="W49" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="X49" t="s">
         <v>253</v>
-      </c>
-      <c r="X49" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="50" spans="1:24" ht="105" x14ac:dyDescent="0.25">
@@ -3782,13 +3781,13 @@
         <v>30</v>
       </c>
       <c r="C50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D50" t="s">
         <v>255</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>256</v>
-      </c>
-      <c r="E50" t="s">
-        <v>257</v>
       </c>
       <c r="F50" t="s">
         <v>53</v>
@@ -3797,10 +3796,10 @@
         <v>248</v>
       </c>
       <c r="J50" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K50" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="L50" t="s">
         <v>242</v>
@@ -3809,7 +3808,7 @@
         <v>251</v>
       </c>
       <c r="S50" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="T50" t="s">
         <v>37</v>
@@ -3821,7 +3820,7 @@
         <v>252</v>
       </c>
       <c r="W50" s="1" t="s">
-        <v>261</v>
+        <v>381</v>
       </c>
     </row>
     <row r="51" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -3832,13 +3831,13 @@
         <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D51" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E51" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F51" t="s">
         <v>53</v>
@@ -3847,10 +3846,10 @@
         <v>248</v>
       </c>
       <c r="J51" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K51" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L51" t="s">
         <v>242</v>
@@ -3879,19 +3878,19 @@
         <v>30</v>
       </c>
       <c r="C52" t="s">
+        <v>264</v>
+      </c>
+      <c r="D52" t="s">
+        <v>265</v>
+      </c>
+      <c r="E52" t="s">
+        <v>265</v>
+      </c>
+      <c r="F52" t="s">
+        <v>53</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="D52" t="s">
-        <v>267</v>
-      </c>
-      <c r="E52" t="s">
-        <v>267</v>
-      </c>
-      <c r="F52" t="s">
-        <v>53</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="J52" t="s">
         <v>76</v>
@@ -3917,13 +3916,13 @@
         <v>30</v>
       </c>
       <c r="C53" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D53" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E53" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F53" t="s">
         <v>53</v>
@@ -3932,10 +3931,10 @@
         <v>248</v>
       </c>
       <c r="J53" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K53" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L53" t="s">
         <v>242</v>
@@ -3964,13 +3963,13 @@
         <v>30</v>
       </c>
       <c r="C54" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D54" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E54" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F54" t="s">
         <v>53</v>
@@ -3979,10 +3978,10 @@
         <v>248</v>
       </c>
       <c r="J54" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K54" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L54" t="s">
         <v>242</v>
@@ -4011,13 +4010,13 @@
         <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D55" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E55" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F55" t="s">
         <v>53</v>
@@ -4026,10 +4025,10 @@
         <v>248</v>
       </c>
       <c r="J55" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="K55" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="Q55" t="s">
         <v>251</v>
@@ -4055,13 +4054,13 @@
         <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D56" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E56" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F56" t="s">
         <v>53</v>
@@ -4070,10 +4069,10 @@
         <v>248</v>
       </c>
       <c r="J56" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K56" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q56" t="s">
         <v>251</v>
@@ -4099,13 +4098,13 @@
         <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D57" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E57" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F57" t="s">
         <v>53</v>
@@ -4114,10 +4113,10 @@
         <v>248</v>
       </c>
       <c r="J57" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="K57" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="Q57" t="s">
         <v>251</v>
@@ -4143,13 +4142,13 @@
         <v>30</v>
       </c>
       <c r="C58" t="s">
+        <v>287</v>
+      </c>
+      <c r="D58" t="s">
+        <v>288</v>
+      </c>
+      <c r="E58" t="s">
         <v>289</v>
-      </c>
-      <c r="D58" t="s">
-        <v>290</v>
-      </c>
-      <c r="E58" t="s">
-        <v>291</v>
       </c>
       <c r="F58" t="s">
         <v>53</v>
@@ -4181,13 +4180,13 @@
         <v>30</v>
       </c>
       <c r="C59" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D59" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E59" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F59" t="s">
         <v>53</v>
@@ -4216,13 +4215,13 @@
         <v>30</v>
       </c>
       <c r="C60" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D60" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E60" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F60" t="s">
         <v>53</v>
@@ -4251,13 +4250,13 @@
         <v>30</v>
       </c>
       <c r="C61" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D61" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E61" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F61" t="s">
         <v>53</v>
@@ -4286,13 +4285,13 @@
         <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D62" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E62" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F62" t="s">
         <v>53</v>
@@ -4321,25 +4320,25 @@
         <v>30</v>
       </c>
       <c r="C63" t="s">
+        <v>298</v>
+      </c>
+      <c r="D63" t="s">
+        <v>299</v>
+      </c>
+      <c r="E63" t="s">
+        <v>299</v>
+      </c>
+      <c r="F63" t="s">
+        <v>53</v>
+      </c>
+      <c r="J63" t="s">
         <v>300</v>
       </c>
-      <c r="D63" t="s">
+      <c r="K63" t="s">
         <v>301</v>
       </c>
-      <c r="E63" t="s">
-        <v>301</v>
-      </c>
-      <c r="F63" t="s">
-        <v>53</v>
-      </c>
-      <c r="J63" t="s">
+      <c r="L63" t="s">
         <v>302</v>
-      </c>
-      <c r="K63" t="s">
-        <v>303</v>
-      </c>
-      <c r="L63" t="s">
-        <v>304</v>
       </c>
       <c r="T63" t="s">
         <v>37</v>
@@ -4362,13 +4361,13 @@
         <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D64" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E64" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F64" t="s">
         <v>53</v>
@@ -4397,25 +4396,25 @@
         <v>30</v>
       </c>
       <c r="C65" t="s">
+        <v>305</v>
+      </c>
+      <c r="D65" t="s">
+        <v>306</v>
+      </c>
+      <c r="E65" t="s">
+        <v>306</v>
+      </c>
+      <c r="F65" t="s">
+        <v>53</v>
+      </c>
+      <c r="J65" t="s">
         <v>307</v>
       </c>
-      <c r="D65" t="s">
+      <c r="K65" t="s">
         <v>308</v>
       </c>
-      <c r="E65" t="s">
-        <v>308</v>
-      </c>
-      <c r="F65" t="s">
-        <v>53</v>
-      </c>
-      <c r="J65" t="s">
+      <c r="L65" t="s">
         <v>309</v>
-      </c>
-      <c r="K65" t="s">
-        <v>310</v>
-      </c>
-      <c r="L65" t="s">
-        <v>311</v>
       </c>
       <c r="T65" t="s">
         <v>37</v>
@@ -4438,19 +4437,19 @@
         <v>30</v>
       </c>
       <c r="C66" t="s">
+        <v>310</v>
+      </c>
+      <c r="D66" t="s">
+        <v>311</v>
+      </c>
+      <c r="E66" t="s">
+        <v>311</v>
+      </c>
+      <c r="F66" t="s">
+        <v>53</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="D66" t="s">
-        <v>313</v>
-      </c>
-      <c r="E66" t="s">
-        <v>313</v>
-      </c>
-      <c r="F66" t="s">
-        <v>53</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="J66" t="s">
         <v>76</v>
@@ -4476,28 +4475,28 @@
         <v>30</v>
       </c>
       <c r="C67" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D67" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E67" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F67" t="s">
         <v>93</v>
       </c>
       <c r="G67" t="s">
+        <v>315</v>
+      </c>
+      <c r="J67" t="s">
+        <v>316</v>
+      </c>
+      <c r="K67" t="s">
         <v>317</v>
       </c>
-      <c r="J67" t="s">
+      <c r="L67" t="s">
         <v>318</v>
-      </c>
-      <c r="K67" t="s">
-        <v>319</v>
-      </c>
-      <c r="L67" t="s">
-        <v>320</v>
       </c>
       <c r="T67" t="s">
         <v>37</v>
@@ -4520,28 +4519,28 @@
         <v>30</v>
       </c>
       <c r="C68" t="s">
+        <v>319</v>
+      </c>
+      <c r="D68" t="s">
+        <v>320</v>
+      </c>
+      <c r="E68" t="s">
+        <v>320</v>
+      </c>
+      <c r="F68" t="s">
+        <v>53</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D68" t="s">
-        <v>322</v>
-      </c>
-      <c r="E68" t="s">
-        <v>322</v>
-      </c>
-      <c r="F68" t="s">
-        <v>53</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>323</v>
-      </c>
       <c r="J68" t="s">
+        <v>316</v>
+      </c>
+      <c r="K68" t="s">
+        <v>317</v>
+      </c>
+      <c r="L68" t="s">
         <v>318</v>
-      </c>
-      <c r="K68" t="s">
-        <v>319</v>
-      </c>
-      <c r="L68" t="s">
-        <v>320</v>
       </c>
       <c r="T68" t="s">
         <v>37</v>
@@ -4553,7 +4552,7 @@
         <v>252</v>
       </c>
       <c r="W68" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="69" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -4564,33 +4563,33 @@
         <v>30</v>
       </c>
       <c r="C69" t="s">
+        <v>323</v>
+      </c>
+      <c r="D69" t="s">
+        <v>324</v>
+      </c>
+      <c r="E69" t="s">
+        <v>324</v>
+      </c>
+      <c r="F69" t="s">
+        <v>53</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="D69" t="s">
-        <v>326</v>
-      </c>
-      <c r="E69" t="s">
-        <v>326</v>
-      </c>
-      <c r="F69" t="s">
-        <v>53</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="J69" t="s">
         <v>76</v>
       </c>
-      <c r="T69" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U69" s="4" t="s">
+      <c r="T69" t="s">
+        <v>70</v>
+      </c>
+      <c r="U69" t="s">
         <v>77</v>
       </c>
-      <c r="V69" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W69" s="4" t="s">
+      <c r="V69" t="s">
+        <v>70</v>
+      </c>
+      <c r="W69" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4602,33 +4601,33 @@
         <v>30</v>
       </c>
       <c r="C70" t="s">
+        <v>326</v>
+      </c>
+      <c r="D70" t="s">
+        <v>327</v>
+      </c>
+      <c r="E70" t="s">
+        <v>327</v>
+      </c>
+      <c r="F70" t="s">
+        <v>53</v>
+      </c>
+      <c r="I70" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="D70" t="s">
-        <v>329</v>
-      </c>
-      <c r="E70" t="s">
-        <v>329</v>
-      </c>
-      <c r="F70" t="s">
-        <v>53</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>330</v>
       </c>
       <c r="J70" t="s">
         <v>76</v>
       </c>
-      <c r="T70" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U70" s="4" t="s">
+      <c r="T70" t="s">
+        <v>70</v>
+      </c>
+      <c r="U70" t="s">
         <v>77</v>
       </c>
-      <c r="V70" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W70" s="4" t="s">
+      <c r="V70" t="s">
+        <v>70</v>
+      </c>
+      <c r="W70" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4640,33 +4639,33 @@
         <v>30</v>
       </c>
       <c r="C71" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D71" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E71" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F71" t="s">
         <v>53</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J71" t="s">
         <v>76</v>
       </c>
-      <c r="T71" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U71" s="4" t="s">
+      <c r="T71" t="s">
+        <v>70</v>
+      </c>
+      <c r="U71" t="s">
         <v>77</v>
       </c>
-      <c r="V71" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W71" s="4" t="s">
+      <c r="V71" t="s">
+        <v>70</v>
+      </c>
+      <c r="W71" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4678,33 +4677,33 @@
         <v>30</v>
       </c>
       <c r="C72" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D72" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E72" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F72" t="s">
         <v>53</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J72" t="s">
         <v>76</v>
       </c>
-      <c r="T72" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U72" s="4" t="s">
+      <c r="T72" t="s">
+        <v>70</v>
+      </c>
+      <c r="U72" t="s">
         <v>77</v>
       </c>
-      <c r="V72" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W72" s="4" t="s">
+      <c r="V72" t="s">
+        <v>70</v>
+      </c>
+      <c r="W72" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4716,33 +4715,33 @@
         <v>30</v>
       </c>
       <c r="C73" t="s">
+        <v>333</v>
+      </c>
+      <c r="D73" t="s">
+        <v>334</v>
+      </c>
+      <c r="E73" t="s">
         <v>335</v>
       </c>
-      <c r="D73" t="s">
+      <c r="F73" t="s">
+        <v>53</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="E73" t="s">
-        <v>337</v>
-      </c>
-      <c r="F73" t="s">
-        <v>53</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="J73" t="s">
         <v>76</v>
       </c>
-      <c r="T73" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U73" s="4" t="s">
+      <c r="T73" t="s">
+        <v>70</v>
+      </c>
+      <c r="U73" t="s">
         <v>77</v>
       </c>
-      <c r="V73" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W73" s="4" t="s">
+      <c r="V73" t="s">
+        <v>70</v>
+      </c>
+      <c r="W73" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4754,33 +4753,33 @@
         <v>30</v>
       </c>
       <c r="C74" t="s">
+        <v>337</v>
+      </c>
+      <c r="D74" t="s">
+        <v>338</v>
+      </c>
+      <c r="E74" t="s">
         <v>339</v>
       </c>
-      <c r="D74" t="s">
+      <c r="F74" t="s">
+        <v>53</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="E74" t="s">
-        <v>341</v>
-      </c>
-      <c r="F74" t="s">
-        <v>53</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="J74" t="s">
         <v>76</v>
       </c>
-      <c r="T74" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U74" s="4" t="s">
+      <c r="T74" t="s">
+        <v>70</v>
+      </c>
+      <c r="U74" t="s">
         <v>77</v>
       </c>
-      <c r="V74" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W74" s="4" t="s">
+      <c r="V74" t="s">
+        <v>70</v>
+      </c>
+      <c r="W74" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4792,33 +4791,33 @@
         <v>30</v>
       </c>
       <c r="C75" t="s">
+        <v>341</v>
+      </c>
+      <c r="D75" t="s">
+        <v>342</v>
+      </c>
+      <c r="E75" t="s">
         <v>343</v>
       </c>
-      <c r="D75" t="s">
+      <c r="F75" t="s">
+        <v>53</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="E75" t="s">
-        <v>345</v>
-      </c>
-      <c r="F75" t="s">
-        <v>53</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>346</v>
       </c>
       <c r="J75" t="s">
         <v>76</v>
       </c>
-      <c r="T75" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U75" s="4" t="s">
+      <c r="T75" t="s">
+        <v>70</v>
+      </c>
+      <c r="U75" t="s">
         <v>77</v>
       </c>
-      <c r="V75" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W75" s="4" t="s">
+      <c r="V75" t="s">
+        <v>70</v>
+      </c>
+      <c r="W75" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4830,33 +4829,33 @@
         <v>30</v>
       </c>
       <c r="C76" t="s">
+        <v>345</v>
+      </c>
+      <c r="D76" t="s">
+        <v>346</v>
+      </c>
+      <c r="E76" t="s">
         <v>347</v>
       </c>
-      <c r="D76" t="s">
-        <v>348</v>
-      </c>
-      <c r="E76" t="s">
-        <v>349</v>
-      </c>
       <c r="F76" t="s">
         <v>53</v>
       </c>
       <c r="G76" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J76" t="s">
         <v>76</v>
       </c>
-      <c r="T76" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U76" s="4" t="s">
+      <c r="T76" t="s">
+        <v>70</v>
+      </c>
+      <c r="U76" t="s">
         <v>77</v>
       </c>
-      <c r="V76" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W76" s="4" t="s">
+      <c r="V76" t="s">
+        <v>70</v>
+      </c>
+      <c r="W76" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4868,33 +4867,33 @@
         <v>30</v>
       </c>
       <c r="C77" t="s">
+        <v>348</v>
+      </c>
+      <c r="D77" t="s">
+        <v>349</v>
+      </c>
+      <c r="E77" t="s">
         <v>350</v>
       </c>
-      <c r="D77" t="s">
+      <c r="F77" t="s">
+        <v>53</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="E77" t="s">
-        <v>352</v>
-      </c>
-      <c r="F77" t="s">
-        <v>53</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="J77" t="s">
         <v>76</v>
       </c>
-      <c r="T77" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U77" s="4" t="s">
+      <c r="T77" t="s">
+        <v>70</v>
+      </c>
+      <c r="U77" t="s">
         <v>77</v>
       </c>
-      <c r="V77" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W77" s="4" t="s">
+      <c r="V77" t="s">
+        <v>70</v>
+      </c>
+      <c r="W77" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4906,33 +4905,33 @@
         <v>30</v>
       </c>
       <c r="C78" t="s">
+        <v>352</v>
+      </c>
+      <c r="D78" t="s">
+        <v>353</v>
+      </c>
+      <c r="E78" t="s">
         <v>354</v>
       </c>
-      <c r="D78" t="s">
+      <c r="F78" t="s">
+        <v>53</v>
+      </c>
+      <c r="I78" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="E78" t="s">
-        <v>356</v>
-      </c>
-      <c r="F78" t="s">
-        <v>53</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>357</v>
       </c>
       <c r="J78" t="s">
         <v>76</v>
       </c>
-      <c r="T78" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U78" s="4" t="s">
+      <c r="T78" t="s">
+        <v>70</v>
+      </c>
+      <c r="U78" t="s">
         <v>77</v>
       </c>
-      <c r="V78" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W78" s="4" t="s">
+      <c r="V78" t="s">
+        <v>70</v>
+      </c>
+      <c r="W78" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4944,33 +4943,33 @@
         <v>30</v>
       </c>
       <c r="C79" t="s">
+        <v>356</v>
+      </c>
+      <c r="D79" t="s">
+        <v>357</v>
+      </c>
+      <c r="E79" t="s">
+        <v>357</v>
+      </c>
+      <c r="F79" t="s">
+        <v>53</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="D79" t="s">
-        <v>359</v>
-      </c>
-      <c r="E79" t="s">
-        <v>359</v>
-      </c>
-      <c r="F79" t="s">
-        <v>53</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="J79" t="s">
         <v>76</v>
       </c>
-      <c r="T79" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U79" s="4" t="s">
+      <c r="T79" t="s">
+        <v>70</v>
+      </c>
+      <c r="U79" t="s">
         <v>77</v>
       </c>
-      <c r="V79" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W79" s="4" t="s">
+      <c r="V79" t="s">
+        <v>70</v>
+      </c>
+      <c r="W79" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4982,13 +4981,13 @@
         <v>30</v>
       </c>
       <c r="C80" t="s">
+        <v>359</v>
+      </c>
+      <c r="D80" t="s">
+        <v>360</v>
+      </c>
+      <c r="E80" t="s">
         <v>361</v>
-      </c>
-      <c r="D80" t="s">
-        <v>362</v>
-      </c>
-      <c r="E80" t="s">
-        <v>363</v>
       </c>
       <c r="F80" t="s">
         <v>53</v>
@@ -4999,16 +4998,16 @@
       <c r="J80" t="s">
         <v>76</v>
       </c>
-      <c r="T80" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U80" s="4" t="s">
+      <c r="T80" t="s">
+        <v>70</v>
+      </c>
+      <c r="U80" t="s">
         <v>77</v>
       </c>
-      <c r="V80" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W80" s="4" t="s">
+      <c r="V80" t="s">
+        <v>70</v>
+      </c>
+      <c r="W80" t="s">
         <v>70</v>
       </c>
     </row>
@@ -5020,13 +5019,13 @@
         <v>30</v>
       </c>
       <c r="C81" t="s">
+        <v>362</v>
+      </c>
+      <c r="D81" t="s">
+        <v>363</v>
+      </c>
+      <c r="E81" t="s">
         <v>364</v>
-      </c>
-      <c r="D81" t="s">
-        <v>365</v>
-      </c>
-      <c r="E81" t="s">
-        <v>366</v>
       </c>
       <c r="F81" t="s">
         <v>53</v>
@@ -5037,16 +5036,16 @@
       <c r="J81" t="s">
         <v>76</v>
       </c>
-      <c r="T81" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U81" s="4" t="s">
+      <c r="T81" t="s">
+        <v>70</v>
+      </c>
+      <c r="U81" t="s">
         <v>77</v>
       </c>
-      <c r="V81" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W81" s="4" t="s">
+      <c r="V81" t="s">
+        <v>70</v>
+      </c>
+      <c r="W81" t="s">
         <v>70</v>
       </c>
     </row>
@@ -5058,13 +5057,13 @@
         <v>30</v>
       </c>
       <c r="C82" t="s">
+        <v>365</v>
+      </c>
+      <c r="D82" t="s">
+        <v>366</v>
+      </c>
+      <c r="E82" t="s">
         <v>367</v>
-      </c>
-      <c r="D82" t="s">
-        <v>368</v>
-      </c>
-      <c r="E82" t="s">
-        <v>369</v>
       </c>
       <c r="F82" t="s">
         <v>53</v>
@@ -5075,16 +5074,16 @@
       <c r="J82" t="s">
         <v>76</v>
       </c>
-      <c r="T82" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U82" s="4" t="s">
+      <c r="T82" t="s">
+        <v>70</v>
+      </c>
+      <c r="U82" t="s">
         <v>77</v>
       </c>
-      <c r="V82" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W82" s="4" t="s">
+      <c r="V82" t="s">
+        <v>70</v>
+      </c>
+      <c r="W82" t="s">
         <v>70</v>
       </c>
     </row>
@@ -5096,13 +5095,13 @@
         <v>30</v>
       </c>
       <c r="C83" t="s">
+        <v>368</v>
+      </c>
+      <c r="D83" t="s">
+        <v>369</v>
+      </c>
+      <c r="E83" t="s">
         <v>370</v>
-      </c>
-      <c r="D83" t="s">
-        <v>371</v>
-      </c>
-      <c r="E83" t="s">
-        <v>372</v>
       </c>
       <c r="F83" t="s">
         <v>53</v>
@@ -5110,16 +5109,16 @@
       <c r="J83" t="s">
         <v>76</v>
       </c>
-      <c r="T83" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U83" s="4" t="s">
+      <c r="T83" t="s">
+        <v>70</v>
+      </c>
+      <c r="U83" t="s">
         <v>77</v>
       </c>
-      <c r="V83" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W83" s="4" t="s">
+      <c r="V83" t="s">
+        <v>70</v>
+      </c>
+      <c r="W83" t="s">
         <v>70</v>
       </c>
     </row>
@@ -5131,33 +5130,33 @@
         <v>30</v>
       </c>
       <c r="C84" t="s">
+        <v>371</v>
+      </c>
+      <c r="D84" t="s">
+        <v>372</v>
+      </c>
+      <c r="E84" t="s">
         <v>373</v>
       </c>
-      <c r="D84" t="s">
+      <c r="F84" t="s">
+        <v>53</v>
+      </c>
+      <c r="G84" t="s">
         <v>374</v>
-      </c>
-      <c r="E84" t="s">
-        <v>375</v>
-      </c>
-      <c r="F84" t="s">
-        <v>53</v>
-      </c>
-      <c r="G84" t="s">
-        <v>376</v>
       </c>
       <c r="J84" t="s">
         <v>76</v>
       </c>
-      <c r="T84" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U84" s="4" t="s">
+      <c r="T84" t="s">
+        <v>70</v>
+      </c>
+      <c r="U84" t="s">
         <v>77</v>
       </c>
-      <c r="V84" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W84" s="4" t="s">
+      <c r="V84" t="s">
+        <v>70</v>
+      </c>
+      <c r="W84" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
put medication variables as undetermined for now
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHK.xlsx
+++ b/data_processing_elements-CHK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9C9C79-9A4C-4756-8D6F-D15D0559BEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14A2821-870D-4E7F-ACB1-D1C3E9829D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DEB00B6D-B98D-41B0-8753-944EECEBCC27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="385">
   <si>
     <t>index</t>
   </si>
@@ -1278,6 +1278,12 @@
 MHSTRK == 1 | MHHEART == 1 | MHBP == 1 ~ 1L;
 MHSTRK == 0 &amp; MHHEART == 0 &amp; MHBP == 0 ~ 0L;
 ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>undetermined</t>
+  </si>
+  <si>
+    <t>variables will soon be ready</t>
   </si>
 </sst>
 </file>
@@ -1670,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90857538-AC28-4A1B-9DA3-1B4B03EDEFF4}">
   <dimension ref="A1:AD84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H47" workbookViewId="0">
-      <selection activeCell="W49" sqref="W49"/>
+    <sheetView tabSelected="1" topLeftCell="H49" workbookViewId="0">
+      <selection activeCell="W52" sqref="W52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4034,16 +4040,19 @@
         <v>251</v>
       </c>
       <c r="T55" t="s">
-        <v>37</v>
+        <v>383</v>
       </c>
       <c r="U55" t="s">
-        <v>38</v>
+        <v>383</v>
       </c>
       <c r="V55" t="s">
-        <v>63</v>
+        <v>383</v>
       </c>
       <c r="W55" t="s">
-        <v>63</v>
+        <v>383</v>
+      </c>
+      <c r="X55" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4078,16 +4087,19 @@
         <v>251</v>
       </c>
       <c r="T56" t="s">
-        <v>37</v>
+        <v>383</v>
       </c>
       <c r="U56" t="s">
-        <v>38</v>
+        <v>383</v>
       </c>
       <c r="V56" t="s">
-        <v>63</v>
+        <v>383</v>
       </c>
       <c r="W56" t="s">
-        <v>63</v>
+        <v>383</v>
+      </c>
+      <c r="X56" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4122,16 +4134,19 @@
         <v>251</v>
       </c>
       <c r="T57" t="s">
-        <v>37</v>
+        <v>383</v>
       </c>
       <c r="U57" t="s">
-        <v>38</v>
+        <v>383</v>
       </c>
       <c r="V57" t="s">
-        <v>63</v>
+        <v>383</v>
       </c>
       <c r="W57" t="s">
-        <v>63</v>
+        <v>383</v>
+      </c>
+      <c r="X57" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
correction completion date, cvd, body fat % method
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHK.xlsx
+++ b/data_processing_elements-CHK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14A2821-870D-4E7F-ACB1-D1C3E9829D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E132A5-B700-4147-BE90-1C826701E5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DEB00B6D-B98D-41B0-8753-944EECEBCC27}"/>
   </bookViews>
@@ -185,9 +185,6 @@
     <t>operation</t>
   </si>
   <si>
-    <t>format(as.Date(Assessment_Date, format = "%m-%d-%Y"), "%Y-%m-%d")</t>
-  </si>
-  <si>
     <t>sdc_sex</t>
   </si>
   <si>
@@ -1263,9 +1260,6 @@
     <t>paste</t>
   </si>
   <si>
-    <t>"BIA (Inbody770)"</t>
-  </si>
-  <si>
     <t>information provided by the study</t>
   </si>
   <si>
@@ -1274,16 +1268,22 @@
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
+    <t>undetermined</t>
+  </si>
+  <si>
+    <t>variables will soon be ready</t>
+  </si>
+  <si>
+    <t>ifelse(!is.na(PBF),"BIA (Inbody770)",NA)</t>
+  </si>
+  <si>
+    <t>as.Date(Assessment_Date, format = "%m/%d/%Y")</t>
+  </si>
+  <si>
     <t>case_when(
-MHSTRK == 1 | MHHEART == 1 | MHBP == 1 ~ 1L;
-MHSTRK == 0 &amp; MHHEART == 0 &amp; MHBP == 0 ~ 0L;
+MHSTRK == 1 | MHHEART == 1 | MHBP == 1 | MHHTOT == 1 ~ 1L;
+MHSTRK == 0 &amp; MHHEART == 0 &amp; MHBP == 0 &amp; MHHTOT == 0 ~ 0L;
 ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>undetermined</t>
-  </si>
-  <si>
-    <t>variables will soon be ready</t>
   </si>
 </sst>
 </file>
@@ -1676,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90857538-AC28-4A1B-9DA3-1B4B03EDEFF4}">
   <dimension ref="A1:AD84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H49" workbookViewId="0">
-      <selection activeCell="W52" sqref="W52"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,7 +1866,7 @@
         <v>48</v>
       </c>
       <c r="W3" t="s">
-        <v>49</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -1877,31 +1877,31 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
         <v>50</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>51</v>
       </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
       <c r="F4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" t="s">
         <v>54</v>
       </c>
-      <c r="J4" t="s">
-        <v>55</v>
-      </c>
       <c r="K4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L4" t="s">
         <v>36</v>
       </c>
       <c r="Q4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T4" t="s">
         <v>37</v>
@@ -1910,10 +1910,10 @@
         <v>47</v>
       </c>
       <c r="V4" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" t="s">
         <v>57</v>
-      </c>
-      <c r="W4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -1924,25 +1924,25 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
         <v>59</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>60</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" t="s">
         <v>61</v>
       </c>
-      <c r="F5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" t="s">
-        <v>62</v>
-      </c>
       <c r="J5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s">
         <v>36</v>
@@ -1954,10 +1954,10 @@
         <v>38</v>
       </c>
       <c r="V5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="60" x14ac:dyDescent="0.25">
@@ -1968,40 +1968,40 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
         <v>64</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>65</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" t="s">
         <v>67</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>68</v>
-      </c>
-      <c r="K6" t="s">
-        <v>69</v>
       </c>
       <c r="L6" t="s">
         <v>36</v>
       </c>
       <c r="T6" t="s">
+        <v>69</v>
+      </c>
+      <c r="U6" t="s">
         <v>70</v>
       </c>
-      <c r="U6" t="s">
-        <v>71</v>
-      </c>
       <c r="V6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="135" x14ac:dyDescent="0.25">
@@ -2012,34 +2012,34 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>73</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" t="s">
         <v>75</v>
       </c>
-      <c r="J7" t="s">
+      <c r="T7" t="s">
+        <v>69</v>
+      </c>
+      <c r="U7" t="s">
         <v>76</v>
       </c>
-      <c r="T7" t="s">
-        <v>70</v>
-      </c>
-      <c r="U7" t="s">
-        <v>77</v>
-      </c>
       <c r="V7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -2050,31 +2050,31 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
         <v>78</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>79</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" t="s">
         <v>81</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>82</v>
-      </c>
-      <c r="K8" t="s">
-        <v>83</v>
       </c>
       <c r="L8" t="s">
         <v>36</v>
       </c>
       <c r="Q8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T8" t="s">
         <v>37</v>
@@ -2083,10 +2083,10 @@
         <v>47</v>
       </c>
       <c r="V8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -2097,34 +2097,34 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
         <v>86</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>87</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="J9" t="s">
+        <v>75</v>
+      </c>
+      <c r="T9" t="s">
+        <v>69</v>
+      </c>
+      <c r="U9" t="s">
         <v>76</v>
       </c>
-      <c r="T9" t="s">
-        <v>70</v>
-      </c>
-      <c r="U9" t="s">
-        <v>77</v>
-      </c>
       <c r="V9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -2135,31 +2135,31 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
         <v>90</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>91</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>92</v>
       </c>
-      <c r="F10" t="s">
-        <v>93</v>
-      </c>
       <c r="J10" t="s">
+        <v>75</v>
+      </c>
+      <c r="T10" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10" t="s">
         <v>76</v>
       </c>
-      <c r="T10" t="s">
-        <v>70</v>
-      </c>
-      <c r="U10" t="s">
-        <v>77</v>
-      </c>
       <c r="V10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -2170,31 +2170,31 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
         <v>94</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>95</v>
-      </c>
-      <c r="E11" t="s">
-        <v>96</v>
       </c>
       <c r="F11" t="s">
         <v>34</v>
       </c>
       <c r="J11" t="s">
+        <v>75</v>
+      </c>
+      <c r="T11" t="s">
+        <v>69</v>
+      </c>
+      <c r="U11" t="s">
         <v>76</v>
       </c>
-      <c r="T11" t="s">
-        <v>70</v>
-      </c>
-      <c r="U11" t="s">
-        <v>77</v>
-      </c>
       <c r="V11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -2205,31 +2205,31 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
         <v>97</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>98</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="J12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" t="s">
         <v>82</v>
-      </c>
-      <c r="K12" t="s">
-        <v>83</v>
       </c>
       <c r="L12" t="s">
         <v>36</v>
       </c>
       <c r="Q12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T12" t="s">
         <v>37</v>
@@ -2238,10 +2238,10 @@
         <v>47</v>
       </c>
       <c r="V12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="45" x14ac:dyDescent="0.25">
@@ -2252,43 +2252,43 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" t="s">
         <v>102</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>103</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F13" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" t="s">
         <v>105</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>106</v>
-      </c>
-      <c r="K13" t="s">
-        <v>107</v>
       </c>
       <c r="L13" t="s">
         <v>36</v>
       </c>
       <c r="Q13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T13" t="s">
+        <v>69</v>
+      </c>
+      <c r="U13" t="s">
         <v>70</v>
       </c>
-      <c r="U13" t="s">
-        <v>71</v>
-      </c>
       <c r="V13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -2299,31 +2299,31 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" t="s">
         <v>109</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>110</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="J14" t="s">
+        <v>105</v>
+      </c>
+      <c r="K14" t="s">
         <v>106</v>
-      </c>
-      <c r="K14" t="s">
-        <v>107</v>
       </c>
       <c r="L14" t="s">
         <v>36</v>
       </c>
       <c r="Q14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T14" t="s">
         <v>37</v>
@@ -2332,10 +2332,10 @@
         <v>47</v>
       </c>
       <c r="V14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -2346,22 +2346,22 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" t="s">
         <v>113</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E15" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="J15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T15" t="s">
         <v>37</v>
@@ -2370,13 +2370,13 @@
         <v>38</v>
       </c>
       <c r="V15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="W15">
         <v>2</v>
       </c>
       <c r="X15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -2387,28 +2387,28 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" t="s">
         <v>116</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" t="s">
         <v>117</v>
       </c>
-      <c r="E16" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="J16" t="s">
         <v>118</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>119</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>120</v>
-      </c>
-      <c r="L16" t="s">
-        <v>121</v>
       </c>
       <c r="T16" t="s">
         <v>37</v>
@@ -2417,10 +2417,10 @@
         <v>38</v>
       </c>
       <c r="V16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2431,28 +2431,28 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" t="s">
         <v>122</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E17" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="J17" t="s">
+        <v>118</v>
+      </c>
+      <c r="K17" t="s">
         <v>119</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>120</v>
-      </c>
-      <c r="L17" t="s">
-        <v>121</v>
       </c>
       <c r="T17" t="s">
         <v>37</v>
@@ -2464,7 +2464,7 @@
         <v>48</v>
       </c>
       <c r="W17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -2475,28 +2475,28 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
         <v>126</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" t="s">
         <v>127</v>
       </c>
-      <c r="E18" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="J18" t="s">
         <v>128</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>129</v>
       </c>
-      <c r="K18" t="s">
-        <v>130</v>
-      </c>
       <c r="L18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T18" t="s">
         <v>37</v>
@@ -2505,10 +2505,10 @@
         <v>38</v>
       </c>
       <c r="V18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2519,28 +2519,28 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" t="s">
         <v>131</v>
       </c>
-      <c r="D19" t="s">
-        <v>132</v>
-      </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J19" t="s">
+        <v>128</v>
+      </c>
+      <c r="K19" t="s">
         <v>129</v>
       </c>
-      <c r="K19" t="s">
-        <v>130</v>
-      </c>
       <c r="L19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T19" t="s">
         <v>37</v>
@@ -2552,7 +2552,7 @@
         <v>48</v>
       </c>
       <c r="W19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="75" x14ac:dyDescent="0.25">
@@ -2563,28 +2563,28 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" t="s">
         <v>134</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" t="s">
         <v>135</v>
       </c>
-      <c r="E20" t="s">
-        <v>135</v>
-      </c>
-      <c r="F20" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="J20" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="L20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T20" t="s">
         <v>37</v>
@@ -2596,7 +2596,7 @@
         <v>48</v>
       </c>
       <c r="W20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -2607,34 +2607,34 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" t="s">
         <v>139</v>
       </c>
-      <c r="D21" t="s">
-        <v>140</v>
-      </c>
       <c r="E21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J21" t="s">
+        <v>75</v>
+      </c>
+      <c r="T21" t="s">
+        <v>69</v>
+      </c>
+      <c r="U21" t="s">
         <v>76</v>
       </c>
-      <c r="T21" t="s">
-        <v>70</v>
-      </c>
-      <c r="U21" t="s">
-        <v>77</v>
-      </c>
       <c r="V21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2645,34 +2645,34 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" t="s">
         <v>141</v>
       </c>
-      <c r="D22" t="s">
-        <v>142</v>
-      </c>
       <c r="E22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J22" t="s">
+        <v>75</v>
+      </c>
+      <c r="T22" t="s">
+        <v>69</v>
+      </c>
+      <c r="U22" t="s">
         <v>76</v>
       </c>
-      <c r="T22" t="s">
-        <v>70</v>
-      </c>
-      <c r="U22" t="s">
-        <v>77</v>
-      </c>
       <c r="V22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -2683,28 +2683,28 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" t="s">
         <v>143</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" t="s">
         <v>144</v>
       </c>
-      <c r="E23" t="s">
-        <v>144</v>
-      </c>
-      <c r="F23" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="J23" t="s">
         <v>145</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>146</v>
       </c>
-      <c r="K23" t="s">
-        <v>147</v>
-      </c>
       <c r="L23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T23" t="s">
         <v>37</v>
@@ -2713,10 +2713,10 @@
         <v>38</v>
       </c>
       <c r="V23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
@@ -2727,25 +2727,25 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" t="s">
         <v>148</v>
       </c>
-      <c r="D24" t="s">
-        <v>149</v>
-      </c>
       <c r="E24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F24" t="s">
         <v>34</v>
       </c>
       <c r="J24" t="s">
+        <v>145</v>
+      </c>
+      <c r="K24" t="s">
         <v>146</v>
       </c>
-      <c r="K24" t="s">
-        <v>147</v>
-      </c>
       <c r="L24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T24" t="s">
         <v>37</v>
@@ -2754,10 +2754,10 @@
         <v>38</v>
       </c>
       <c r="V24" t="s">
-        <v>378</v>
+        <v>48</v>
       </c>
       <c r="W24" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -2768,28 +2768,28 @@
         <v>30</v>
       </c>
       <c r="C25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" t="s">
         <v>150</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>151</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" t="s">
         <v>152</v>
       </c>
-      <c r="F25" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="J25" t="s">
         <v>153</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>154</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>155</v>
-      </c>
-      <c r="L25" t="s">
-        <v>156</v>
       </c>
       <c r="T25" t="s">
         <v>37</v>
@@ -2798,10 +2798,10 @@
         <v>38</v>
       </c>
       <c r="V25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -2812,28 +2812,28 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" t="s">
         <v>157</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>158</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" t="s">
+        <v>152</v>
+      </c>
+      <c r="J26" t="s">
         <v>159</v>
       </c>
-      <c r="F26" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" t="s">
-        <v>153</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>160</v>
       </c>
-      <c r="K26" t="s">
-        <v>161</v>
-      </c>
       <c r="L26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T26" t="s">
         <v>37</v>
@@ -2842,10 +2842,10 @@
         <v>38</v>
       </c>
       <c r="V26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
@@ -2856,28 +2856,28 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" t="s">
         <v>162</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
+        <v>162</v>
+      </c>
+      <c r="F27" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" t="s">
         <v>163</v>
       </c>
-      <c r="E27" t="s">
-        <v>163</v>
-      </c>
-      <c r="F27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="J27" t="s">
         <v>164</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>165</v>
       </c>
-      <c r="K27" t="s">
-        <v>166</v>
-      </c>
       <c r="L27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T27" t="s">
         <v>37</v>
@@ -2886,10 +2886,10 @@
         <v>38</v>
       </c>
       <c r="V27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
@@ -2900,34 +2900,34 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" t="s">
         <v>167</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>167</v>
+      </c>
+      <c r="F28" t="s">
+        <v>92</v>
+      </c>
+      <c r="G28" t="s">
         <v>168</v>
       </c>
-      <c r="E28" t="s">
-        <v>168</v>
-      </c>
-      <c r="F28" t="s">
-        <v>93</v>
-      </c>
-      <c r="G28" t="s">
-        <v>169</v>
-      </c>
       <c r="J28" t="s">
+        <v>75</v>
+      </c>
+      <c r="T28" t="s">
+        <v>69</v>
+      </c>
+      <c r="U28" t="s">
         <v>76</v>
       </c>
-      <c r="T28" t="s">
-        <v>70</v>
-      </c>
-      <c r="U28" t="s">
-        <v>77</v>
-      </c>
       <c r="V28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -2938,34 +2938,34 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" t="s">
         <v>170</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E29" t="s">
-        <v>171</v>
-      </c>
-      <c r="F29" t="s">
-        <v>53</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="J29" t="s">
+        <v>75</v>
+      </c>
+      <c r="T29" t="s">
+        <v>69</v>
+      </c>
+      <c r="U29" t="s">
         <v>76</v>
       </c>
-      <c r="T29" t="s">
-        <v>70</v>
-      </c>
-      <c r="U29" t="s">
-        <v>77</v>
-      </c>
       <c r="V29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
@@ -2976,34 +2976,34 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30" t="s">
         <v>173</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
+        <v>173</v>
+      </c>
+      <c r="F30" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" t="s">
         <v>174</v>
       </c>
-      <c r="E30" t="s">
-        <v>174</v>
-      </c>
-      <c r="F30" t="s">
-        <v>93</v>
-      </c>
-      <c r="G30" t="s">
-        <v>175</v>
-      </c>
       <c r="J30" t="s">
+        <v>75</v>
+      </c>
+      <c r="T30" t="s">
+        <v>69</v>
+      </c>
+      <c r="U30" t="s">
         <v>76</v>
       </c>
-      <c r="T30" t="s">
-        <v>70</v>
-      </c>
-      <c r="U30" t="s">
-        <v>77</v>
-      </c>
       <c r="V30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
@@ -3014,34 +3014,34 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
+        <v>175</v>
+      </c>
+      <c r="D31" t="s">
         <v>176</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" t="s">
         <v>177</v>
       </c>
-      <c r="E31" t="s">
-        <v>177</v>
-      </c>
-      <c r="F31" t="s">
-        <v>93</v>
-      </c>
-      <c r="G31" t="s">
-        <v>178</v>
-      </c>
       <c r="J31" t="s">
+        <v>75</v>
+      </c>
+      <c r="T31" t="s">
+        <v>69</v>
+      </c>
+      <c r="U31" t="s">
         <v>76</v>
       </c>
-      <c r="T31" t="s">
-        <v>70</v>
-      </c>
-      <c r="U31" t="s">
-        <v>77</v>
-      </c>
       <c r="V31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
@@ -3052,34 +3052,34 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
+        <v>178</v>
+      </c>
+      <c r="D32" t="s">
         <v>179</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>179</v>
+      </c>
+      <c r="F32" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" t="s">
         <v>180</v>
       </c>
-      <c r="E32" t="s">
-        <v>180</v>
-      </c>
-      <c r="F32" t="s">
-        <v>93</v>
-      </c>
-      <c r="G32" t="s">
-        <v>181</v>
-      </c>
       <c r="J32" t="s">
+        <v>75</v>
+      </c>
+      <c r="T32" t="s">
+        <v>69</v>
+      </c>
+      <c r="U32" t="s">
         <v>76</v>
       </c>
-      <c r="T32" t="s">
-        <v>70</v>
-      </c>
-      <c r="U32" t="s">
-        <v>77</v>
-      </c>
       <c r="V32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
@@ -3090,34 +3090,34 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
+        <v>181</v>
+      </c>
+      <c r="D33" t="s">
         <v>182</v>
       </c>
-      <c r="D33" t="s">
-        <v>183</v>
-      </c>
       <c r="E33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J33" t="s">
+        <v>75</v>
+      </c>
+      <c r="T33" t="s">
+        <v>69</v>
+      </c>
+      <c r="U33" t="s">
         <v>76</v>
       </c>
-      <c r="T33" t="s">
-        <v>70</v>
-      </c>
-      <c r="U33" t="s">
-        <v>77</v>
-      </c>
       <c r="V33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
@@ -3128,34 +3128,34 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
+        <v>183</v>
+      </c>
+      <c r="D34" t="s">
         <v>184</v>
       </c>
-      <c r="D34" t="s">
-        <v>185</v>
-      </c>
       <c r="E34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J34" t="s">
+        <v>75</v>
+      </c>
+      <c r="T34" t="s">
+        <v>69</v>
+      </c>
+      <c r="U34" t="s">
         <v>76</v>
       </c>
-      <c r="T34" t="s">
-        <v>70</v>
-      </c>
-      <c r="U34" t="s">
-        <v>77</v>
-      </c>
       <c r="V34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
@@ -3166,34 +3166,34 @@
         <v>30</v>
       </c>
       <c r="C35" t="s">
+        <v>185</v>
+      </c>
+      <c r="D35" t="s">
         <v>186</v>
       </c>
-      <c r="D35" t="s">
-        <v>187</v>
-      </c>
       <c r="E35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J35" t="s">
+        <v>75</v>
+      </c>
+      <c r="T35" t="s">
+        <v>69</v>
+      </c>
+      <c r="U35" t="s">
         <v>76</v>
       </c>
-      <c r="T35" t="s">
-        <v>70</v>
-      </c>
-      <c r="U35" t="s">
-        <v>77</v>
-      </c>
       <c r="V35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
@@ -3204,34 +3204,34 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
+        <v>187</v>
+      </c>
+      <c r="D36" t="s">
         <v>188</v>
       </c>
-      <c r="D36" t="s">
-        <v>189</v>
-      </c>
       <c r="E36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J36" t="s">
+        <v>75</v>
+      </c>
+      <c r="T36" t="s">
+        <v>69</v>
+      </c>
+      <c r="U36" t="s">
         <v>76</v>
       </c>
-      <c r="T36" t="s">
-        <v>70</v>
-      </c>
-      <c r="U36" t="s">
-        <v>77</v>
-      </c>
       <c r="V36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
@@ -3242,34 +3242,34 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D37" t="s">
         <v>190</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
+        <v>190</v>
+      </c>
+      <c r="F37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G37" t="s">
         <v>191</v>
       </c>
-      <c r="E37" t="s">
-        <v>191</v>
-      </c>
-      <c r="F37" t="s">
-        <v>93</v>
-      </c>
-      <c r="G37" t="s">
-        <v>192</v>
-      </c>
       <c r="J37" t="s">
+        <v>75</v>
+      </c>
+      <c r="T37" t="s">
+        <v>69</v>
+      </c>
+      <c r="U37" t="s">
         <v>76</v>
       </c>
-      <c r="T37" t="s">
-        <v>70</v>
-      </c>
-      <c r="U37" t="s">
-        <v>77</v>
-      </c>
       <c r="V37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
@@ -3280,34 +3280,34 @@
         <v>30</v>
       </c>
       <c r="C38" t="s">
+        <v>192</v>
+      </c>
+      <c r="D38" t="s">
         <v>193</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>194</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G38" t="s">
         <v>195</v>
       </c>
-      <c r="F38" t="s">
-        <v>93</v>
-      </c>
-      <c r="G38" t="s">
-        <v>196</v>
-      </c>
       <c r="J38" t="s">
+        <v>75</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U38" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="U38" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="V38" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -3318,34 +3318,34 @@
         <v>30</v>
       </c>
       <c r="C39" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" t="s">
         <v>197</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>198</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
+        <v>52</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F39" t="s">
-        <v>53</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="J39" t="s">
+        <v>75</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U39" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T39" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="U39" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="V39" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W39" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
@@ -3356,34 +3356,34 @@
         <v>30</v>
       </c>
       <c r="C40" t="s">
+        <v>200</v>
+      </c>
+      <c r="D40" t="s">
         <v>201</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>202</v>
       </c>
-      <c r="E40" t="s">
-        <v>203</v>
-      </c>
       <c r="F40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G40" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J40" t="s">
+        <v>75</v>
+      </c>
+      <c r="T40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U40" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T40" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="U40" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="V40" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W40" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -3394,34 +3394,34 @@
         <v>30</v>
       </c>
       <c r="C41" t="s">
+        <v>203</v>
+      </c>
+      <c r="D41" t="s">
         <v>204</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>205</v>
       </c>
-      <c r="E41" t="s">
-        <v>206</v>
-      </c>
       <c r="F41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J41" t="s">
+        <v>75</v>
+      </c>
+      <c r="T41" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U41" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T41" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="U41" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="V41" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W41" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
@@ -3432,34 +3432,34 @@
         <v>30</v>
       </c>
       <c r="C42" t="s">
+        <v>206</v>
+      </c>
+      <c r="D42" t="s">
         <v>207</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
+        <v>207</v>
+      </c>
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" t="s">
         <v>208</v>
       </c>
-      <c r="E42" t="s">
-        <v>208</v>
-      </c>
-      <c r="F42" t="s">
-        <v>93</v>
-      </c>
-      <c r="G42" t="s">
-        <v>209</v>
-      </c>
       <c r="J42" t="s">
+        <v>75</v>
+      </c>
+      <c r="T42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U42" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T42" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="U42" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="V42" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W42" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
@@ -3470,34 +3470,34 @@
         <v>30</v>
       </c>
       <c r="C43" t="s">
+        <v>209</v>
+      </c>
+      <c r="D43" t="s">
         <v>210</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>211</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" t="s">
         <v>212</v>
       </c>
-      <c r="F43" t="s">
-        <v>93</v>
-      </c>
-      <c r="G43" t="s">
-        <v>213</v>
-      </c>
       <c r="J43" t="s">
+        <v>75</v>
+      </c>
+      <c r="T43" t="s">
+        <v>69</v>
+      </c>
+      <c r="U43" t="s">
         <v>76</v>
       </c>
-      <c r="T43" t="s">
-        <v>70</v>
-      </c>
-      <c r="U43" t="s">
-        <v>77</v>
-      </c>
       <c r="V43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -3508,31 +3508,31 @@
         <v>30</v>
       </c>
       <c r="C44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D44" t="s">
         <v>214</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>214</v>
+      </c>
+      <c r="F44" t="s">
+        <v>52</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E44" t="s">
-        <v>215</v>
-      </c>
-      <c r="F44" t="s">
-        <v>53</v>
-      </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" t="s">
         <v>216</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
         <v>217</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>218</v>
       </c>
-      <c r="L44" t="s">
+      <c r="Q44" t="s">
         <v>219</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>220</v>
       </c>
       <c r="T44" t="s">
         <v>37</v>
@@ -3541,13 +3541,13 @@
         <v>47</v>
       </c>
       <c r="V44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W44" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="X44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -3558,31 +3558,31 @@
         <v>30</v>
       </c>
       <c r="C45" t="s">
+        <v>221</v>
+      </c>
+      <c r="D45" t="s">
         <v>222</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>223</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
+        <v>52</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="F45" t="s">
-        <v>53</v>
-      </c>
-      <c r="I45" s="1" t="s">
+      <c r="J45" t="s">
         <v>225</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>226</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q45" t="s">
         <v>227</v>
-      </c>
-      <c r="L45" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>228</v>
       </c>
       <c r="T45" t="s">
         <v>37</v>
@@ -3591,10 +3591,10 @@
         <v>47</v>
       </c>
       <c r="V45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -3605,31 +3605,31 @@
         <v>30</v>
       </c>
       <c r="C46" t="s">
+        <v>229</v>
+      </c>
+      <c r="D46" t="s">
         <v>230</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
+        <v>230</v>
+      </c>
+      <c r="F46" t="s">
+        <v>52</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E46" t="s">
-        <v>231</v>
-      </c>
-      <c r="F46" t="s">
-        <v>53</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>232</v>
-      </c>
       <c r="J46" t="s">
+        <v>225</v>
+      </c>
+      <c r="K46" t="s">
         <v>226</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q46" t="s">
         <v>227</v>
-      </c>
-      <c r="L46" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>228</v>
       </c>
       <c r="T46" t="s">
         <v>37</v>
@@ -3638,10 +3638,10 @@
         <v>47</v>
       </c>
       <c r="V46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
@@ -3652,34 +3652,34 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
+        <v>233</v>
+      </c>
+      <c r="D47" t="s">
         <v>234</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>234</v>
+      </c>
+      <c r="F47" t="s">
+        <v>52</v>
+      </c>
+      <c r="G47" t="s">
         <v>235</v>
       </c>
-      <c r="E47" t="s">
-        <v>235</v>
-      </c>
-      <c r="F47" t="s">
-        <v>53</v>
-      </c>
-      <c r="G47" t="s">
-        <v>236</v>
-      </c>
       <c r="J47" t="s">
+        <v>75</v>
+      </c>
+      <c r="T47" t="s">
+        <v>69</v>
+      </c>
+      <c r="U47" t="s">
         <v>76</v>
       </c>
-      <c r="T47" t="s">
-        <v>70</v>
-      </c>
-      <c r="U47" t="s">
-        <v>77</v>
-      </c>
       <c r="V47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:24" ht="120" x14ac:dyDescent="0.25">
@@ -3690,31 +3690,31 @@
         <v>30</v>
       </c>
       <c r="C48" t="s">
+        <v>236</v>
+      </c>
+      <c r="D48" t="s">
         <v>237</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>237</v>
+      </c>
+      <c r="F48" t="s">
+        <v>52</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E48" t="s">
-        <v>238</v>
-      </c>
-      <c r="F48" t="s">
-        <v>53</v>
-      </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" t="s">
         <v>239</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>240</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>241</v>
       </c>
-      <c r="L48" t="s">
+      <c r="Q48" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="T48" t="s">
         <v>37</v>
@@ -3723,10 +3723,10 @@
         <v>47</v>
       </c>
       <c r="V48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W48" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" spans="1:24" ht="240" x14ac:dyDescent="0.25">
@@ -3737,31 +3737,31 @@
         <v>30</v>
       </c>
       <c r="C49" t="s">
+        <v>244</v>
+      </c>
+      <c r="D49" t="s">
         <v>245</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>246</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
+        <v>52</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="F49" t="s">
-        <v>53</v>
-      </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q49" t="s">
         <v>250</v>
-      </c>
-      <c r="L49" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>251</v>
       </c>
       <c r="T49" t="s">
         <v>37</v>
@@ -3770,13 +3770,13 @@
         <v>47</v>
       </c>
       <c r="V49" t="s">
+        <v>251</v>
+      </c>
+      <c r="W49" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="X49" t="s">
         <v>252</v>
-      </c>
-      <c r="W49" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="X49" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:24" ht="105" x14ac:dyDescent="0.25">
@@ -3787,34 +3787,34 @@
         <v>30</v>
       </c>
       <c r="C50" t="s">
+        <v>253</v>
+      </c>
+      <c r="D50" t="s">
         <v>254</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>255</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
+        <v>52</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J50" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="F50" t="s">
-        <v>53</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="J50" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="L50" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>250</v>
+      </c>
+      <c r="S50" t="s">
         <v>258</v>
-      </c>
-      <c r="L50" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>251</v>
-      </c>
-      <c r="S50" t="s">
-        <v>259</v>
       </c>
       <c r="T50" t="s">
         <v>37</v>
@@ -3823,10 +3823,10 @@
         <v>47</v>
       </c>
       <c r="V50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W50" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="51" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -3837,31 +3837,31 @@
         <v>30</v>
       </c>
       <c r="C51" t="s">
+        <v>259</v>
+      </c>
+      <c r="D51" t="s">
         <v>260</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
+        <v>260</v>
+      </c>
+      <c r="F51" t="s">
+        <v>52</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J51" t="s">
         <v>261</v>
       </c>
-      <c r="E51" t="s">
-        <v>261</v>
-      </c>
-      <c r="F51" t="s">
-        <v>53</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>262</v>
       </c>
-      <c r="K51" t="s">
-        <v>263</v>
-      </c>
       <c r="L51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q51" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T51" t="s">
         <v>37</v>
@@ -3870,10 +3870,10 @@
         <v>38</v>
       </c>
       <c r="V51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -3884,34 +3884,34 @@
         <v>30</v>
       </c>
       <c r="C52" t="s">
+        <v>263</v>
+      </c>
+      <c r="D52" t="s">
         <v>264</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
+        <v>264</v>
+      </c>
+      <c r="F52" t="s">
+        <v>52</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E52" t="s">
-        <v>265</v>
-      </c>
-      <c r="F52" t="s">
-        <v>53</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="J52" t="s">
+        <v>75</v>
+      </c>
+      <c r="T52" t="s">
+        <v>69</v>
+      </c>
+      <c r="U52" t="s">
         <v>76</v>
       </c>
-      <c r="T52" t="s">
-        <v>70</v>
-      </c>
-      <c r="U52" t="s">
-        <v>77</v>
-      </c>
       <c r="V52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -3922,31 +3922,31 @@
         <v>30</v>
       </c>
       <c r="C53" t="s">
+        <v>266</v>
+      </c>
+      <c r="D53" t="s">
         <v>267</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
+        <v>267</v>
+      </c>
+      <c r="F53" t="s">
+        <v>52</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J53" t="s">
         <v>268</v>
       </c>
-      <c r="E53" t="s">
-        <v>268</v>
-      </c>
-      <c r="F53" t="s">
-        <v>53</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>269</v>
       </c>
-      <c r="K53" t="s">
-        <v>270</v>
-      </c>
       <c r="L53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q53" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T53" t="s">
         <v>37</v>
@@ -3955,10 +3955,10 @@
         <v>38</v>
       </c>
       <c r="V53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -3969,31 +3969,31 @@
         <v>30</v>
       </c>
       <c r="C54" t="s">
+        <v>270</v>
+      </c>
+      <c r="D54" t="s">
         <v>271</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
+        <v>271</v>
+      </c>
+      <c r="F54" t="s">
+        <v>52</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J54" t="s">
         <v>272</v>
       </c>
-      <c r="E54" t="s">
-        <v>272</v>
-      </c>
-      <c r="F54" t="s">
-        <v>53</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>273</v>
       </c>
-      <c r="K54" t="s">
-        <v>274</v>
-      </c>
       <c r="L54" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q54" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T54" t="s">
         <v>37</v>
@@ -4002,10 +4002,10 @@
         <v>38</v>
       </c>
       <c r="V54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4016,43 +4016,43 @@
         <v>30</v>
       </c>
       <c r="C55" t="s">
+        <v>274</v>
+      </c>
+      <c r="D55" t="s">
         <v>275</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
+        <v>275</v>
+      </c>
+      <c r="F55" t="s">
+        <v>52</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J55" t="s">
         <v>276</v>
       </c>
-      <c r="E55" t="s">
-        <v>276</v>
-      </c>
-      <c r="F55" t="s">
-        <v>53</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="J55" t="s">
+      <c r="K55" t="s">
         <v>277</v>
       </c>
-      <c r="K55" t="s">
-        <v>278</v>
-      </c>
       <c r="Q55" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T55" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="U55" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="V55" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="W55" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="X55" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4063,43 +4063,43 @@
         <v>30</v>
       </c>
       <c r="C56" t="s">
+        <v>278</v>
+      </c>
+      <c r="D56" t="s">
         <v>279</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
+        <v>279</v>
+      </c>
+      <c r="F56" t="s">
+        <v>52</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J56" t="s">
         <v>280</v>
       </c>
-      <c r="E56" t="s">
-        <v>280</v>
-      </c>
-      <c r="F56" t="s">
-        <v>53</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="J56" t="s">
+      <c r="K56" t="s">
         <v>281</v>
       </c>
-      <c r="K56" t="s">
-        <v>282</v>
-      </c>
       <c r="Q56" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T56" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="U56" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="V56" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="W56" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="X56" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4110,43 +4110,43 @@
         <v>30</v>
       </c>
       <c r="C57" t="s">
+        <v>282</v>
+      </c>
+      <c r="D57" t="s">
         <v>283</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
+        <v>283</v>
+      </c>
+      <c r="F57" t="s">
+        <v>52</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J57" t="s">
         <v>284</v>
       </c>
-      <c r="E57" t="s">
-        <v>284</v>
-      </c>
-      <c r="F57" t="s">
-        <v>53</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="J57" t="s">
+      <c r="K57" t="s">
         <v>285</v>
       </c>
-      <c r="K57" t="s">
-        <v>286</v>
-      </c>
       <c r="Q57" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T57" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="U57" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="V57" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="W57" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="X57" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4157,34 +4157,34 @@
         <v>30</v>
       </c>
       <c r="C58" t="s">
+        <v>286</v>
+      </c>
+      <c r="D58" t="s">
         <v>287</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>288</v>
       </c>
-      <c r="E58" t="s">
-        <v>289</v>
-      </c>
       <c r="F58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J58" t="s">
+        <v>75</v>
+      </c>
+      <c r="T58" t="s">
+        <v>69</v>
+      </c>
+      <c r="U58" t="s">
         <v>76</v>
       </c>
-      <c r="T58" t="s">
-        <v>70</v>
-      </c>
-      <c r="U58" t="s">
-        <v>77</v>
-      </c>
       <c r="V58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
@@ -4195,31 +4195,31 @@
         <v>30</v>
       </c>
       <c r="C59" t="s">
+        <v>289</v>
+      </c>
+      <c r="D59" t="s">
         <v>290</v>
       </c>
-      <c r="D59" t="s">
-        <v>291</v>
-      </c>
       <c r="E59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J59" t="s">
+        <v>75</v>
+      </c>
+      <c r="T59" t="s">
+        <v>69</v>
+      </c>
+      <c r="U59" t="s">
         <v>76</v>
       </c>
-      <c r="T59" t="s">
-        <v>70</v>
-      </c>
-      <c r="U59" t="s">
-        <v>77</v>
-      </c>
       <c r="V59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
@@ -4230,31 +4230,31 @@
         <v>30</v>
       </c>
       <c r="C60" t="s">
+        <v>291</v>
+      </c>
+      <c r="D60" t="s">
         <v>292</v>
       </c>
-      <c r="D60" t="s">
-        <v>293</v>
-      </c>
       <c r="E60" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J60" t="s">
+        <v>75</v>
+      </c>
+      <c r="T60" t="s">
+        <v>69</v>
+      </c>
+      <c r="U60" t="s">
         <v>76</v>
       </c>
-      <c r="T60" t="s">
-        <v>70</v>
-      </c>
-      <c r="U60" t="s">
-        <v>77</v>
-      </c>
       <c r="V60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
@@ -4265,31 +4265,31 @@
         <v>30</v>
       </c>
       <c r="C61" t="s">
+        <v>293</v>
+      </c>
+      <c r="D61" t="s">
         <v>294</v>
       </c>
-      <c r="D61" t="s">
-        <v>295</v>
-      </c>
       <c r="E61" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F61" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J61" t="s">
+        <v>75</v>
+      </c>
+      <c r="T61" t="s">
+        <v>69</v>
+      </c>
+      <c r="U61" t="s">
         <v>76</v>
       </c>
-      <c r="T61" t="s">
-        <v>70</v>
-      </c>
-      <c r="U61" t="s">
-        <v>77</v>
-      </c>
       <c r="V61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
@@ -4300,31 +4300,31 @@
         <v>30</v>
       </c>
       <c r="C62" t="s">
+        <v>295</v>
+      </c>
+      <c r="D62" t="s">
         <v>296</v>
       </c>
-      <c r="D62" t="s">
-        <v>297</v>
-      </c>
       <c r="E62" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J62" t="s">
+        <v>75</v>
+      </c>
+      <c r="T62" t="s">
+        <v>69</v>
+      </c>
+      <c r="U62" t="s">
         <v>76</v>
       </c>
-      <c r="T62" t="s">
-        <v>70</v>
-      </c>
-      <c r="U62" t="s">
-        <v>77</v>
-      </c>
       <c r="V62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
@@ -4335,25 +4335,25 @@
         <v>30</v>
       </c>
       <c r="C63" t="s">
+        <v>297</v>
+      </c>
+      <c r="D63" t="s">
         <v>298</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
+        <v>298</v>
+      </c>
+      <c r="F63" t="s">
+        <v>52</v>
+      </c>
+      <c r="J63" t="s">
         <v>299</v>
       </c>
-      <c r="E63" t="s">
-        <v>299</v>
-      </c>
-      <c r="F63" t="s">
-        <v>53</v>
-      </c>
-      <c r="J63" t="s">
+      <c r="K63" t="s">
         <v>300</v>
       </c>
-      <c r="K63" t="s">
+      <c r="L63" t="s">
         <v>301</v>
-      </c>
-      <c r="L63" t="s">
-        <v>302</v>
       </c>
       <c r="T63" t="s">
         <v>37</v>
@@ -4362,10 +4362,10 @@
         <v>38</v>
       </c>
       <c r="V63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
@@ -4376,31 +4376,31 @@
         <v>30</v>
       </c>
       <c r="C64" t="s">
+        <v>302</v>
+      </c>
+      <c r="D64" t="s">
         <v>303</v>
       </c>
-      <c r="D64" t="s">
-        <v>304</v>
-      </c>
       <c r="E64" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F64" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J64" t="s">
+        <v>75</v>
+      </c>
+      <c r="T64" t="s">
+        <v>69</v>
+      </c>
+      <c r="U64" t="s">
         <v>76</v>
       </c>
-      <c r="T64" t="s">
-        <v>70</v>
-      </c>
-      <c r="U64" t="s">
-        <v>77</v>
-      </c>
       <c r="V64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
@@ -4411,25 +4411,25 @@
         <v>30</v>
       </c>
       <c r="C65" t="s">
+        <v>304</v>
+      </c>
+      <c r="D65" t="s">
         <v>305</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
+        <v>305</v>
+      </c>
+      <c r="F65" t="s">
+        <v>52</v>
+      </c>
+      <c r="J65" t="s">
         <v>306</v>
       </c>
-      <c r="E65" t="s">
-        <v>306</v>
-      </c>
-      <c r="F65" t="s">
-        <v>53</v>
-      </c>
-      <c r="J65" t="s">
+      <c r="K65" t="s">
         <v>307</v>
       </c>
-      <c r="K65" t="s">
+      <c r="L65" t="s">
         <v>308</v>
-      </c>
-      <c r="L65" t="s">
-        <v>309</v>
       </c>
       <c r="T65" t="s">
         <v>37</v>
@@ -4438,10 +4438,10 @@
         <v>38</v>
       </c>
       <c r="V65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -4452,34 +4452,34 @@
         <v>30</v>
       </c>
       <c r="C66" t="s">
+        <v>309</v>
+      </c>
+      <c r="D66" t="s">
         <v>310</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
+        <v>310</v>
+      </c>
+      <c r="F66" t="s">
+        <v>52</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="E66" t="s">
-        <v>311</v>
-      </c>
-      <c r="F66" t="s">
-        <v>53</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="J66" t="s">
+        <v>75</v>
+      </c>
+      <c r="T66" t="s">
+        <v>69</v>
+      </c>
+      <c r="U66" t="s">
         <v>76</v>
       </c>
-      <c r="T66" t="s">
-        <v>70</v>
-      </c>
-      <c r="U66" t="s">
-        <v>77</v>
-      </c>
       <c r="V66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
@@ -4490,28 +4490,28 @@
         <v>30</v>
       </c>
       <c r="C67" t="s">
+        <v>312</v>
+      </c>
+      <c r="D67" t="s">
         <v>313</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
+        <v>313</v>
+      </c>
+      <c r="F67" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" t="s">
         <v>314</v>
       </c>
-      <c r="E67" t="s">
-        <v>314</v>
-      </c>
-      <c r="F67" t="s">
-        <v>93</v>
-      </c>
-      <c r="G67" t="s">
+      <c r="J67" t="s">
         <v>315</v>
       </c>
-      <c r="J67" t="s">
+      <c r="K67" t="s">
         <v>316</v>
       </c>
-      <c r="K67" t="s">
+      <c r="L67" t="s">
         <v>317</v>
-      </c>
-      <c r="L67" t="s">
-        <v>318</v>
       </c>
       <c r="T67" t="s">
         <v>37</v>
@@ -4520,10 +4520,10 @@
         <v>47</v>
       </c>
       <c r="V67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:23" ht="165" x14ac:dyDescent="0.25">
@@ -4534,28 +4534,28 @@
         <v>30</v>
       </c>
       <c r="C68" t="s">
+        <v>318</v>
+      </c>
+      <c r="D68" t="s">
         <v>319</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
+        <v>319</v>
+      </c>
+      <c r="F68" t="s">
+        <v>52</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E68" t="s">
-        <v>320</v>
-      </c>
-      <c r="F68" t="s">
-        <v>53</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>321</v>
-      </c>
       <c r="J68" t="s">
+        <v>315</v>
+      </c>
+      <c r="K68" t="s">
         <v>316</v>
       </c>
-      <c r="K68" t="s">
+      <c r="L68" t="s">
         <v>317</v>
-      </c>
-      <c r="L68" t="s">
-        <v>318</v>
       </c>
       <c r="T68" t="s">
         <v>37</v>
@@ -4564,10 +4564,10 @@
         <v>47</v>
       </c>
       <c r="V68" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W68" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="69" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -4578,34 +4578,34 @@
         <v>30</v>
       </c>
       <c r="C69" t="s">
+        <v>322</v>
+      </c>
+      <c r="D69" t="s">
         <v>323</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
+        <v>323</v>
+      </c>
+      <c r="F69" t="s">
+        <v>52</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="E69" t="s">
-        <v>324</v>
-      </c>
-      <c r="F69" t="s">
-        <v>53</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="J69" t="s">
+        <v>75</v>
+      </c>
+      <c r="T69" t="s">
+        <v>69</v>
+      </c>
+      <c r="U69" t="s">
         <v>76</v>
       </c>
-      <c r="T69" t="s">
-        <v>70</v>
-      </c>
-      <c r="U69" t="s">
-        <v>77</v>
-      </c>
       <c r="V69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -4616,34 +4616,34 @@
         <v>30</v>
       </c>
       <c r="C70" t="s">
+        <v>325</v>
+      </c>
+      <c r="D70" t="s">
         <v>326</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
+        <v>326</v>
+      </c>
+      <c r="F70" t="s">
+        <v>52</v>
+      </c>
+      <c r="I70" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E70" t="s">
-        <v>327</v>
-      </c>
-      <c r="F70" t="s">
-        <v>53</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="J70" t="s">
+        <v>75</v>
+      </c>
+      <c r="T70" t="s">
+        <v>69</v>
+      </c>
+      <c r="U70" t="s">
         <v>76</v>
       </c>
-      <c r="T70" t="s">
-        <v>70</v>
-      </c>
-      <c r="U70" t="s">
-        <v>77</v>
-      </c>
       <c r="V70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -4654,34 +4654,34 @@
         <v>30</v>
       </c>
       <c r="C71" t="s">
+        <v>328</v>
+      </c>
+      <c r="D71" t="s">
         <v>329</v>
       </c>
-      <c r="D71" t="s">
-        <v>330</v>
-      </c>
       <c r="E71" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F71" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J71" t="s">
+        <v>75</v>
+      </c>
+      <c r="T71" t="s">
+        <v>69</v>
+      </c>
+      <c r="U71" t="s">
         <v>76</v>
       </c>
-      <c r="T71" t="s">
-        <v>70</v>
-      </c>
-      <c r="U71" t="s">
-        <v>77</v>
-      </c>
       <c r="V71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -4692,34 +4692,34 @@
         <v>30</v>
       </c>
       <c r="C72" t="s">
+        <v>330</v>
+      </c>
+      <c r="D72" t="s">
         <v>331</v>
       </c>
-      <c r="D72" t="s">
-        <v>332</v>
-      </c>
       <c r="E72" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J72" t="s">
+        <v>75</v>
+      </c>
+      <c r="T72" t="s">
+        <v>69</v>
+      </c>
+      <c r="U72" t="s">
         <v>76</v>
       </c>
-      <c r="T72" t="s">
-        <v>70</v>
-      </c>
-      <c r="U72" t="s">
-        <v>77</v>
-      </c>
       <c r="V72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:23" ht="165" x14ac:dyDescent="0.25">
@@ -4730,34 +4730,34 @@
         <v>30</v>
       </c>
       <c r="C73" t="s">
+        <v>332</v>
+      </c>
+      <c r="D73" t="s">
         <v>333</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>334</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
+        <v>52</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="F73" t="s">
-        <v>53</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="J73" t="s">
+        <v>75</v>
+      </c>
+      <c r="T73" t="s">
+        <v>69</v>
+      </c>
+      <c r="U73" t="s">
         <v>76</v>
       </c>
-      <c r="T73" t="s">
-        <v>70</v>
-      </c>
-      <c r="U73" t="s">
-        <v>77</v>
-      </c>
       <c r="V73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -4768,34 +4768,34 @@
         <v>30</v>
       </c>
       <c r="C74" t="s">
+        <v>336</v>
+      </c>
+      <c r="D74" t="s">
         <v>337</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>338</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
+        <v>52</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="F74" t="s">
-        <v>53</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>340</v>
-      </c>
       <c r="J74" t="s">
+        <v>75</v>
+      </c>
+      <c r="T74" t="s">
+        <v>69</v>
+      </c>
+      <c r="U74" t="s">
         <v>76</v>
       </c>
-      <c r="T74" t="s">
-        <v>70</v>
-      </c>
-      <c r="U74" t="s">
-        <v>77</v>
-      </c>
       <c r="V74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -4806,34 +4806,34 @@
         <v>30</v>
       </c>
       <c r="C75" t="s">
+        <v>340</v>
+      </c>
+      <c r="D75" t="s">
         <v>341</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>342</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
+        <v>52</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="F75" t="s">
-        <v>53</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>344</v>
-      </c>
       <c r="J75" t="s">
+        <v>75</v>
+      </c>
+      <c r="T75" t="s">
+        <v>69</v>
+      </c>
+      <c r="U75" t="s">
         <v>76</v>
       </c>
-      <c r="T75" t="s">
-        <v>70</v>
-      </c>
-      <c r="U75" t="s">
-        <v>77</v>
-      </c>
       <c r="V75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.25">
@@ -4844,34 +4844,34 @@
         <v>30</v>
       </c>
       <c r="C76" t="s">
+        <v>344</v>
+      </c>
+      <c r="D76" t="s">
         <v>345</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>346</v>
       </c>
-      <c r="E76" t="s">
-        <v>347</v>
-      </c>
       <c r="F76" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G76" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J76" t="s">
+        <v>75</v>
+      </c>
+      <c r="T76" t="s">
+        <v>69</v>
+      </c>
+      <c r="U76" t="s">
         <v>76</v>
       </c>
-      <c r="T76" t="s">
-        <v>70</v>
-      </c>
-      <c r="U76" t="s">
-        <v>77</v>
-      </c>
       <c r="V76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -4882,34 +4882,34 @@
         <v>30</v>
       </c>
       <c r="C77" t="s">
+        <v>347</v>
+      </c>
+      <c r="D77" t="s">
         <v>348</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>349</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
+        <v>52</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="F77" t="s">
-        <v>53</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="J77" t="s">
+        <v>75</v>
+      </c>
+      <c r="T77" t="s">
+        <v>69</v>
+      </c>
+      <c r="U77" t="s">
         <v>76</v>
       </c>
-      <c r="T77" t="s">
-        <v>70</v>
-      </c>
-      <c r="U77" t="s">
-        <v>77</v>
-      </c>
       <c r="V77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -4920,34 +4920,34 @@
         <v>30</v>
       </c>
       <c r="C78" t="s">
+        <v>351</v>
+      </c>
+      <c r="D78" t="s">
         <v>352</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>353</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
+        <v>52</v>
+      </c>
+      <c r="I78" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="F78" t="s">
-        <v>53</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="J78" t="s">
+        <v>75</v>
+      </c>
+      <c r="T78" t="s">
+        <v>69</v>
+      </c>
+      <c r="U78" t="s">
         <v>76</v>
       </c>
-      <c r="T78" t="s">
-        <v>70</v>
-      </c>
-      <c r="U78" t="s">
-        <v>77</v>
-      </c>
       <c r="V78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -4958,34 +4958,34 @@
         <v>30</v>
       </c>
       <c r="C79" t="s">
+        <v>355</v>
+      </c>
+      <c r="D79" t="s">
         <v>356</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
+        <v>356</v>
+      </c>
+      <c r="F79" t="s">
+        <v>52</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="E79" t="s">
-        <v>357</v>
-      </c>
-      <c r="F79" t="s">
-        <v>53</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>358</v>
-      </c>
       <c r="J79" t="s">
+        <v>75</v>
+      </c>
+      <c r="T79" t="s">
+        <v>69</v>
+      </c>
+      <c r="U79" t="s">
         <v>76</v>
       </c>
-      <c r="T79" t="s">
-        <v>70</v>
-      </c>
-      <c r="U79" t="s">
-        <v>77</v>
-      </c>
       <c r="V79" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W79" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -4996,34 +4996,34 @@
         <v>30</v>
       </c>
       <c r="C80" t="s">
+        <v>358</v>
+      </c>
+      <c r="D80" t="s">
         <v>359</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>360</v>
       </c>
-      <c r="E80" t="s">
-        <v>361</v>
-      </c>
       <c r="F80" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J80" t="s">
+        <v>75</v>
+      </c>
+      <c r="T80" t="s">
+        <v>69</v>
+      </c>
+      <c r="U80" t="s">
         <v>76</v>
       </c>
-      <c r="T80" t="s">
-        <v>70</v>
-      </c>
-      <c r="U80" t="s">
-        <v>77</v>
-      </c>
       <c r="V80" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W80" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -5034,34 +5034,34 @@
         <v>30</v>
       </c>
       <c r="C81" t="s">
+        <v>361</v>
+      </c>
+      <c r="D81" t="s">
         <v>362</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>363</v>
       </c>
-      <c r="E81" t="s">
-        <v>364</v>
-      </c>
       <c r="F81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J81" t="s">
+        <v>75</v>
+      </c>
+      <c r="T81" t="s">
+        <v>69</v>
+      </c>
+      <c r="U81" t="s">
         <v>76</v>
       </c>
-      <c r="T81" t="s">
-        <v>70</v>
-      </c>
-      <c r="U81" t="s">
-        <v>77</v>
-      </c>
       <c r="V81" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W81" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -5072,34 +5072,34 @@
         <v>30</v>
       </c>
       <c r="C82" t="s">
+        <v>364</v>
+      </c>
+      <c r="D82" t="s">
         <v>365</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>366</v>
       </c>
-      <c r="E82" t="s">
-        <v>367</v>
-      </c>
       <c r="F82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J82" t="s">
+        <v>75</v>
+      </c>
+      <c r="T82" t="s">
+        <v>69</v>
+      </c>
+      <c r="U82" t="s">
         <v>76</v>
       </c>
-      <c r="T82" t="s">
-        <v>70</v>
-      </c>
-      <c r="U82" t="s">
-        <v>77</v>
-      </c>
       <c r="V82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">
@@ -5110,31 +5110,31 @@
         <v>30</v>
       </c>
       <c r="C83" t="s">
+        <v>367</v>
+      </c>
+      <c r="D83" t="s">
         <v>368</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>369</v>
       </c>
-      <c r="E83" t="s">
-        <v>370</v>
-      </c>
       <c r="F83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J83" t="s">
+        <v>75</v>
+      </c>
+      <c r="T83" t="s">
+        <v>69</v>
+      </c>
+      <c r="U83" t="s">
         <v>76</v>
       </c>
-      <c r="T83" t="s">
-        <v>70</v>
-      </c>
-      <c r="U83" t="s">
-        <v>77</v>
-      </c>
       <c r="V83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.25">
@@ -5145,34 +5145,34 @@
         <v>30</v>
       </c>
       <c r="C84" t="s">
+        <v>370</v>
+      </c>
+      <c r="D84" t="s">
         <v>371</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>372</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F84" t="s">
+        <v>52</v>
+      </c>
+      <c r="G84" t="s">
         <v>373</v>
       </c>
-      <c r="F84" t="s">
-        <v>53</v>
-      </c>
-      <c r="G84" t="s">
-        <v>374</v>
-      </c>
       <c r="J84" t="s">
+        <v>75</v>
+      </c>
+      <c r="T84" t="s">
+        <v>69</v>
+      </c>
+      <c r="U84" t="s">
         <v>76</v>
       </c>
-      <c r="T84" t="s">
-        <v>70</v>
-      </c>
-      <c r="U84" t="s">
-        <v>77</v>
-      </c>
       <c r="V84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding harmo rule medication variables
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHK.xlsx
+++ b/data_processing_elements-CHK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E132A5-B700-4147-BE90-1C826701E5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549FCA07-DF2E-4941-B238-8C18D91920E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DEB00B6D-B98D-41B0-8753-944EECEBCC27}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DEB00B6D-B98D-41B0-8753-944EECEBCC27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="384">
   <si>
     <t>index</t>
   </si>
@@ -1266,9 +1266,6 @@
     <t>case_when(
 MHART == 1 | MHOSTEO == 1 ~ 1L;
 ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>undetermined</t>
   </si>
   <si>
     <t>variables will soon be ready</t>
@@ -1358,7 +1355,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1676,11 +1673,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90857538-AC28-4A1B-9DA3-1B4B03EDEFF4}">
   <dimension ref="A1:AD84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="N52" workbookViewId="0">
+      <selection activeCell="W61" sqref="W61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
@@ -1866,7 +1863,7 @@
         <v>48</v>
       </c>
       <c r="W3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -2757,7 +2754,7 @@
         <v>48</v>
       </c>
       <c r="W24" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -3773,7 +3770,7 @@
         <v>251</v>
       </c>
       <c r="W49" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="X49" t="s">
         <v>252</v>
@@ -4040,19 +4037,19 @@
         <v>250</v>
       </c>
       <c r="T55" t="s">
+        <v>37</v>
+      </c>
+      <c r="U55" t="s">
+        <v>38</v>
+      </c>
+      <c r="V55" t="s">
+        <v>62</v>
+      </c>
+      <c r="W55" t="s">
+        <v>62</v>
+      </c>
+      <c r="X55" t="s">
         <v>380</v>
-      </c>
-      <c r="U55" t="s">
-        <v>380</v>
-      </c>
-      <c r="V55" t="s">
-        <v>380</v>
-      </c>
-      <c r="W55" t="s">
-        <v>380</v>
-      </c>
-      <c r="X55" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4087,19 +4084,19 @@
         <v>250</v>
       </c>
       <c r="T56" t="s">
+        <v>37</v>
+      </c>
+      <c r="U56" t="s">
+        <v>38</v>
+      </c>
+      <c r="V56" t="s">
+        <v>62</v>
+      </c>
+      <c r="W56" t="s">
+        <v>62</v>
+      </c>
+      <c r="X56" t="s">
         <v>380</v>
-      </c>
-      <c r="U56" t="s">
-        <v>380</v>
-      </c>
-      <c r="V56" t="s">
-        <v>380</v>
-      </c>
-      <c r="W56" t="s">
-        <v>380</v>
-      </c>
-      <c r="X56" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4134,19 +4131,19 @@
         <v>250</v>
       </c>
       <c r="T57" t="s">
+        <v>37</v>
+      </c>
+      <c r="U57" t="s">
+        <v>38</v>
+      </c>
+      <c r="V57" t="s">
+        <v>62</v>
+      </c>
+      <c r="W57" t="s">
+        <v>62</v>
+      </c>
+      <c r="X57" t="s">
         <v>380</v>
-      </c>
-      <c r="U57" t="s">
-        <v>380</v>
-      </c>
-      <c r="V57" t="s">
-        <v>380</v>
-      </c>
-      <c r="W57" t="s">
-        <v>380</v>
-      </c>
-      <c r="X57" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="30" x14ac:dyDescent="0.25">

</xml_diff>